<commit_message>
Added Bottle Management and adjusted Risk Management files to new version of TJE.
</commit_message>
<xml_diff>
--- a/risk-log/Risk Log.xlsx
+++ b/risk-log/Risk Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\risk-log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\tje-resources\risk-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721C4A93-D103-4ADC-A8CC-7ED2CE005D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD5EA46-1541-419F-A4C7-4CE1B1C5D552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RiskLog" sheetId="1" r:id="rId1"/>
@@ -5446,7 +5446,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> (https://github.com/bks07/risk-log) and write a Medium article to share it with others. You can find the article "Easy Risk Management with Jira, Confluence, and Excel" at https://medium.com/agileinsider/easy-risk-management-with-jira-confluence-and-excel-c7b2dd13f848. There, you can find everything you need to work with this file.</a:t>
+            <a:t> (https://github.com/bks07/tje-resources) and write a Medium article to share it with others. You can find the article "Easy Risk Management with Jira, Confluence, and Excel" at https://medium.com/agileinsider/easy-risk-management-with-jira-confluence-and-excel-c7b2dd13f848. There, you can find everything you need to work with this file.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0">
             <a:solidFill>
@@ -5646,6 +5646,37 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>2024-03-12 #003 Boris Karl Schlein (VLOOKUP -&gt; XLOOKUP)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2024-09-27 #004 Boris Karl Schlein</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6207,37 +6238,37 @@
   </sheetPr>
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.77734375" customWidth="1"/>
-    <col min="17" max="20" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" customWidth="1"/>
+    <col min="17" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="6" customWidth="1"/>
-    <col min="25" max="25" width="35.44140625" customWidth="1"/>
-    <col min="26" max="26" width="17.44140625" customWidth="1"/>
+    <col min="25" max="25" width="35.42578125" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="str">
         <f>Logic!$B$4</f>
         <v/>
@@ -6272,7 +6303,7 @@
       <c r="S1" s="122"/>
       <c r="T1" s="122"/>
     </row>
-    <row r="2" spans="1:20" ht="89.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="93" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>14</v>
       </c>
@@ -6334,7 +6365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="86" t="s">
         <v>66</v>
       </c>
@@ -6415,7 +6446,7 @@
         <v>i2l3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="92"/>
       <c r="B4" s="87"/>
       <c r="C4" s="91"/>
@@ -6768,17 +6799,17 @@
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="10" width="7.109375" customWidth="1"/>
-    <col min="11" max="11" width="2.88671875" customWidth="1"/>
-    <col min="12" max="17" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="12" max="17" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
@@ -6823,7 +6854,7 @@
       <c r="P2" s="136"/>
       <c r="Q2" s="136"/>
     </row>
-    <row r="3" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="135"/>
       <c r="C3" s="18" t="str">
         <f>MasterData!$A$16</f>
@@ -6882,7 +6913,7 @@
         <v>Critical</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="135"/>
       <c r="C4" s="20" t="str">
         <f>MasterData!$A$15</f>
@@ -6941,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="135"/>
       <c r="C5" s="22" t="str">
         <f>MasterData!$A$14</f>
@@ -6976,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="135"/>
       <c r="C6" s="24" t="str">
         <f>MasterData!$A$13</f>
@@ -7011,7 +7042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="135"/>
       <c r="C7" s="9" t="str">
         <f>MasterData!$A$12</f>
@@ -7046,7 +7077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="135"/>
       <c r="C8" s="137"/>
       <c r="D8" s="137"/>
@@ -7075,7 +7106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="135"/>
       <c r="C9" s="137"/>
       <c r="D9" s="137"/>
@@ -7104,7 +7135,7 @@
         <v>Almost Certain</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="136" t="s">
         <v>23</v>
@@ -7174,15 +7205,15 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="59.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="60.75" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -7208,7 +7239,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="96">
         <v>1</v>
       </c>
@@ -7235,7 +7266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="96">
         <v>32</v>
       </c>
@@ -7285,29 +7316,29 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.6640625" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="87.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="115" t="s">
         <v>70</v>
       </c>
@@ -7363,7 +7394,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="115" t="s">
         <v>66</v>
       </c>
@@ -7410,7 +7441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
       <c r="B3" s="109"/>
       <c r="C3" s="110"/>
@@ -7478,17 +7509,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="106" t="s">
         <v>81</v>
       </c>
@@ -7501,7 +7532,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="106" t="s">
         <v>82</v>
       </c>
@@ -7514,7 +7545,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="106" t="s">
         <v>83</v>
       </c>
@@ -7538,14 +7569,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -7553,7 +7584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -7570,7 +7601,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -7584,7 +7615,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -7593,7 +7624,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -7602,7 +7633,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -7611,7 +7642,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -7620,7 +7651,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -7629,12 +7660,12 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -7645,7 +7676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -7653,7 +7684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -7662,7 +7693,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>59</v>
       </c>
@@ -7671,7 +7702,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -7680,7 +7711,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -7689,7 +7720,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -7698,12 +7729,12 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -7714,7 +7745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -7722,7 +7753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -7730,7 +7761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -7738,7 +7769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -7746,7 +7777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -7754,7 +7785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -7762,12 +7793,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -7778,7 +7809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -7786,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -7794,7 +7825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -7802,7 +7833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -7810,7 +7841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -7818,7 +7849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -7826,7 +7857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -7834,7 +7865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -7842,12 +7873,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -7858,7 +7889,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -7869,7 +7900,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -7880,7 +7911,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -7891,12 +7922,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -7907,7 +7938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -7915,7 +7946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -7923,7 +7954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -7931,12 +7962,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>4</v>
       </c>
@@ -7947,7 +7978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>31</v>
       </c>
@@ -7956,7 +7987,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
@@ -7965,7 +7996,7 @@
       </c>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>33</v>
       </c>
@@ -7974,7 +8005,7 @@
       </c>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>34</v>
       </c>
@@ -7983,17 +8014,17 @@
       </c>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -8007,7 +8038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i0l0</v>
@@ -8022,7 +8053,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i0l1</v>
@@ -8037,7 +8068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i0l2</v>
@@ -8052,7 +8083,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i0l3</v>
@@ -8067,7 +8098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i0l4</v>
@@ -8082,7 +8113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i0l5</v>
@@ -8097,7 +8128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i1l0</v>
@@ -8112,7 +8143,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i1l1</v>
@@ -8127,7 +8158,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i1l2</v>
@@ -8142,7 +8173,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i1l3</v>
@@ -8157,7 +8188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i1l4</v>
@@ -8172,7 +8203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i1l5</v>
@@ -8187,7 +8218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i2l0</v>
@@ -8202,7 +8233,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i2l1</v>
@@ -8217,7 +8248,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i2l2</v>
@@ -8232,7 +8263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i2l3</v>
@@ -8247,7 +8278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i2l4</v>
@@ -8262,7 +8293,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i2l5</v>
@@ -8277,7 +8308,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i3l0</v>
@@ -8292,7 +8323,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i3l1</v>
@@ -8307,7 +8338,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i3l2</v>
@@ -8322,7 +8353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i3l3</v>
@@ -8337,7 +8368,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i3l4</v>
@@ -8352,7 +8383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i3l5</v>
@@ -8367,7 +8398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i4l0</v>
@@ -8382,7 +8413,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i4l1</v>
@@ -8397,7 +8428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i4l2</v>
@@ -8412,7 +8443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i4l3</v>
@@ -8427,7 +8458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i4l4</v>
@@ -8442,7 +8473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i4l5</v>
@@ -8457,7 +8488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i5l0</v>
@@ -8472,7 +8503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i5l1</v>
@@ -8487,7 +8518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i5l2</v>
@@ -8502,7 +8533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i5l3</v>
@@ -8517,7 +8548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i5l4</v>
@@ -8532,7 +8563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</f>
         <v>i5l5</v>
@@ -8578,11 +8609,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>